<commit_message>
change the map and the mapping logic  'code-->flat_，flat_simple,type_ and origin_
</commit_message>
<xml_diff>
--- a/xlsx/out_doc2xl.xlsx
+++ b/xlsx/out_doc2xl.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,20 +466,25 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>单位简称</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>类型</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>地区</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>联系人</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>联系电话</t>
         </is>
@@ -491,8 +496,10 @@
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>1</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>GX-SB-ZJDX</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -516,20 +523,25 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>高校院所</t>
+          <t>ZJDX</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>tel135</t>
         </is>
@@ -541,8 +553,10 @@
           <t>2</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>2</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>GX-SB-XHDX</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -566,20 +580,25 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>高校院所</t>
+          <t>XHDX</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>tel135</t>
         </is>
@@ -591,8 +610,10 @@
           <t>3</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>1</v>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>GX-SB-GYDX</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -611,25 +632,30 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>浙江大学</t>
+          <t>浙江工业大学</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>高校院所</t>
+          <t>GYDX</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>tel135</t>
         </is>
@@ -641,8 +667,10 @@
           <t>4</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>2</v>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>GX-SB-ZJSFDX</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -661,25 +689,30 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>西湖大学</t>
+          <t>浙江师范大学</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>高校院所</t>
+          <t>ZJSFDX</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>tel135</t>
         </is>
@@ -691,8 +724,10 @@
           <t>5</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>3</v>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>GX-SB-NBDX</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -711,25 +746,30 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>浙江工业大学</t>
+          <t>宁波大学</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>高校院所</t>
+          <t>NBDX</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>tel135</t>
         </is>
@@ -738,520 +778,607 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>6</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>需手动添加</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>展品6</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>测试6</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>实物6</t>
-        </is>
-      </c>
+          <t>ZYJY-SX-TDSX</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>zjut</t>
+          <t>天津大学浙江绍兴研究院</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>TDSX</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>省实验室和省级新型研发机构</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>tel136</t>
-        </is>
-      </c>
+          <t>绍兴市</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-ZJDX</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>展品7</t>
+          <t>展品1</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>测试7</t>
+          <t>测试1</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>实物7</t>
+          <t>实物1</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>zjut</t>
+          <t>浙江大学</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>ZJDX</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>tel136</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-XHDX</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>展品8</t>
+          <t>展品2</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>测试8</t>
+          <t>测试2</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>实物8</t>
+          <t>实物2</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>zjut</t>
+          <t>西湖大学</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>XHDX</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>tel136</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-GYDX</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>展品9</t>
+          <t>展品3</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>测试9</t>
+          <t>测试3</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>实物9</t>
+          <t>实物3</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>zjut</t>
+          <t>浙江工业大学</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GYDX</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>tel136</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-ZJSFDX</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>展品10</t>
+          <t>展品4</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>测试10</t>
+          <t>测试4</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>实物10</t>
+          <t>实物4</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>zjut</t>
+          <t>浙江师范大学</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>ZJSFDX</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>tel136</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-NBDX</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>展品5</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>测试5</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>实物5</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>宁波大学</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>NBDX</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-ZJDX</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>展品1</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>测试1</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>实物1</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>浙江大学</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>ZJDX</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-XHDX</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>展品2</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>测试2</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>实物2</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>西湖大学</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>XHDX</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-GYDX</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>展品3</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>测试3</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>实物3</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>浙江工业大学</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GYDX</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>GX-SB-ZJSFDX</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>展品4</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>测试4</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>实物4</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>浙江师范大学</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>ZJSFDX</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>需手动添加</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>省本级</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>test_null</t>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>tel135</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>GX-SB-NBDX</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>展品5</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>测试5</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>实物5</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>宁波大学</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>NBDX</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>高校院所</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>省本级</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>tel135</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
change the type of docx file and map
</commit_message>
<xml_diff>
--- a/xlsx/out_doc2xl.xlsx
+++ b/xlsx/out_doc2xl.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>编码</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>序号</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>编码</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -493,17 +493,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>GX-SB-NBDX</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>GX-SB-ZJDX</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>展品1</t>
+          <t>宁波大学展品1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -513,17 +513,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>实物1</t>
+          <t>实物1，名称正确</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>浙江大学</t>
+          <t>宁波大学</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>ZJDX</t>
+          <t>NBDX</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -550,17 +550,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>GX-SB-NBDX</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>GX-SB-XHDX</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>展品2</t>
+          <t>宁波大学展品2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -570,17 +570,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>实物2</t>
+          <t>实物2，名称正确</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>西湖大学</t>
+          <t>宁波大学</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>XHDX</t>
+          <t>NBDX</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -607,17 +607,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>GX-SB-NBDX</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>GX-SB-GYDX</t>
-        </is>
-      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>展品3</t>
+          <t>宁波大学展品3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -627,17 +627,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>实物3</t>
+          <t>实物3，名称混乱</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>浙江工业大学</t>
+          <t>宁波大学</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>GYDX</t>
+          <t>NBDX</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -664,17 +664,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>GX-SB-NBDX</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>GX-SB-ZJSFDX</t>
-        </is>
-      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>展品4</t>
+          <t>宁波大学展品4</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -684,17 +684,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>实物4</t>
+          <t>实物4，名称混乱</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>浙江师范大学</t>
+          <t>宁波大学</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>ZJSFDX</t>
+          <t>NBDX</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -721,17 +721,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>GX-SB-NBDX</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>5</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>GX-SB-NBDX</t>
-        </is>
-      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>展品5</t>
+          <t>宁波大学展品5</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>实物5</t>
+          <t>实物5，名称混乱</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -778,74 +778,94 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>GX-SB-XHDX</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ZYJY-SX-TDSX</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>西湖大学展品1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>测试1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>实物1，名称正确</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>天津大学浙江绍兴研究院</t>
+          <t>西湖大学</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>TDSX</t>
+          <t>XHDX</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>省实验室和省级新型研发机构</t>
+          <t>高校院所</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>绍兴市</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
+          <t>省本级</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>tel135</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>GX-SB-XHDX</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>GX-SB-ZJDX</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>展品1</t>
+          <t>西湖大学展品2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>测试1</t>
+          <t>测试2</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>实物1</t>
+          <t>实物2，名称正确</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>浙江大学</t>
+          <t>西湖大学</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>ZJDX</t>
+          <t>XHDX</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -872,27 +892,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>GX-SB-XHDX</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>GX-SB-XHDX</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>展品2</t>
+          <t>西湖大学展品3</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>测试2</t>
+          <t>测试3</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>实物2</t>
+          <t>实物3，名称混乱</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -929,37 +949,37 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>GX-SB-XHDX</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>GX-SB-GYDX</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>展品3</t>
+          <t>西湖大学展品4</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>测试3</t>
+          <t>测试4</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>实物3</t>
+          <t>实物4，名称混乱</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>浙江工业大学</t>
+          <t>西湖大学</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>GYDX</t>
+          <t>XHDX</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -986,37 +1006,37 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>GX-SB-XHDX</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>GX-SB-ZJSFDX</t>
+          <t>5</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>展品4</t>
+          <t>西湖大学展品5</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>测试4</t>
+          <t>测试5</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>实物4</t>
+          <t>实物5，名称混乱</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>浙江师范大学</t>
+          <t>西湖大学</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>ZJSFDX</t>
+          <t>XHDX</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1035,348 +1055,6 @@
         </is>
       </c>
       <c r="K11" t="inlineStr">
-        <is>
-          <t>tel135</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>GX-SB-NBDX</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>展品5</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>测试5</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>实物5</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>宁波大学</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>NBDX</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>高校院所</t>
-        </is>
-      </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>省本级</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>tel135</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>GX-SB-ZJDX</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>展品1</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>测试1</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>实物1</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>浙江大学</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>ZJDX</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>高校院所</t>
-        </is>
-      </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>省本级</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>tel135</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>GX-SB-XHDX</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>展品2</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>测试2</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>实物2</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>西湖大学</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>XHDX</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>高校院所</t>
-        </is>
-      </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>省本级</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>tel135</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>GX-SB-GYDX</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>展品3</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>测试3</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>实物3</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>浙江工业大学</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>GYDX</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>高校院所</t>
-        </is>
-      </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>省本级</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>tel135</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>GX-SB-ZJSFDX</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>展品4</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>测试4</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>实物4</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>浙江师范大学</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>ZJSFDX</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>高校院所</t>
-        </is>
-      </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>省本级</t>
-        </is>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>tel135</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>GX-SB-NBDX</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>展品5</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>测试5</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>实物5</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>宁波大学</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>NBDX</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>高校院所</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>省本级</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
         <is>
           <t>tel135</t>
         </is>

</xml_diff>